<commit_message>
Update input for G1 velvet regulatory proteins
</commit_message>
<xml_diff>
--- a/input/G1_velvet_regulatory_proteins.xlsx
+++ b/input/G1_velvet_regulatory_proteins.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lazab\Documents\github\Zoospore-RNA-Analysis\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21E12021-CB3B-4C5D-850B-20DFC0AE79FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9548B39B-275D-4E7B-8AA0-99D5AE5F0033}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4020" yWindow="2475" windowWidth="21600" windowHeight="11175" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -371,7 +371,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:A11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
@@ -391,26 +391,46 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>498890</v>
+        <v>699304</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>459971</v>
+        <v>79256</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>514349</v>
+        <v>498890</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>514348</v>
+        <v>79354</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7">
+        <v>394282</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>459971</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>514349</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>514348</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11">
         <v>223018</v>
       </c>
     </row>

</xml_diff>